<commit_message>
View and Modify recipes html work well
Also, now for every recipe that is created a new directory is created with those two htmls and that would be the place for storing Recipe Photos
</commit_message>
<xml_diff>
--- a/CookItUpWeb/Tasks.xlsx
+++ b/CookItUpWeb/Tasks.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inbal\Documents\GitHub\CookItUp\CookItUpWeb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199971DF-8E63-47D3-8AA2-B3223DDD94AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1 (2)" sheetId="2" r:id="rId1"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="112">
   <si>
     <t>Requirement</t>
   </si>
@@ -312,24 +318,12 @@
     <t>/user/{id}/profile.html</t>
   </si>
   <si>
-    <t>If there is a user, we chek if they are the same as the profile</t>
-  </si>
-  <si>
-    <t>If they are not we allow to follow, block and report</t>
-  </si>
-  <si>
     <t>We show the user's recipes</t>
   </si>
   <si>
     <t>/user/{id}/recipes</t>
   </si>
   <si>
-    <t>We show number of followers</t>
-  </si>
-  <si>
-    <t>/user/{id}/num_followers</t>
-  </si>
-  <si>
     <t>Search recipes</t>
   </si>
   <si>
@@ -348,25 +342,43 @@
     <t>Check if there is an admin</t>
   </si>
   <si>
-    <t>/user/{id}/block</t>
-  </si>
-  <si>
-    <t>/user/{id}/follow</t>
-  </si>
-  <si>
-    <t>/user/{id}/report</t>
-  </si>
-  <si>
     <t>If so, shows the reports</t>
   </si>
   <si>
     <t>If not shows Log in and Sign Up</t>
+  </si>
+  <si>
+    <t>/home/log_out</t>
+  </si>
+  <si>
+    <t>/admin/log_out</t>
+  </si>
+  <si>
+    <t>Show the user's fridge at /user/{id}/fridge.html</t>
+  </si>
+  <si>
+    <t>/user/{id}/fridge returns a list of the ingredients in the fridge</t>
+  </si>
+  <si>
+    <t>al hacer el sign up crear profile.html</t>
+  </si>
+  <si>
+    <t>/admin/log_in y /admin/sign_up</t>
+  </si>
+  <si>
+    <t>doesn't work</t>
+  </si>
+  <si>
+    <t>/recipe/search.html</t>
+  </si>
+  <si>
+    <t>/recipe/{name}/search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -616,24 +628,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -698,9 +697,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -749,8 +745,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -779,31 +778,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1112,27 +1096,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="51.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="51.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="51.7109375" style="2"/>
-    <col min="4" max="16384" width="51.7109375" style="1"/>
+    <col min="1" max="3" width="51.6640625" style="2"/>
+    <col min="4" max="16384" width="51.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1149,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>21</v>
       </c>
@@ -1176,35 +1160,35 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="40"/>
       <c r="B5" s="41"/>
       <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="40"/>
       <c r="B6" s="41"/>
       <c r="C6" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="40"/>
       <c r="B7" s="41"/>
       <c r="C7" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="40"/>
       <c r="B8" s="41"/>
       <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1223,7 +1207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1247,22 +1231,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1270,7 +1254,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1286,27 +1270,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1317,7 +1301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1325,17 +1309,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1350,22 +1334,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="51.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="51.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" style="6" customWidth="1"/>
-    <col min="2" max="3" width="60.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" style="6" customWidth="1"/>
+    <col min="2" max="3" width="60.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="13" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="51.7109375" style="7"/>
+    <col min="5" max="16384" width="51.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>21</v>
       </c>
@@ -1412,7 +1396,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43"/>
       <c r="C5" s="8" t="s">
@@ -1422,28 +1406,28 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="B6" s="43"/>
       <c r="C6" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="43"/>
       <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
       <c r="B8" s="43"/>
       <c r="C8" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1454,7 +1438,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
@@ -1463,7 +1447,7 @@
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
@@ -1472,7 +1456,7 @@
       </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -1481,7 +1465,7 @@
       </c>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -1490,28 +1474,28 @@
       </c>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>12</v>
       </c>
@@ -1520,7 +1504,7 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1529,7 +1513,7 @@
       </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
@@ -1538,35 +1522,35 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
@@ -1577,29 +1561,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>19</v>
       </c>
@@ -1617,148 +1601,148 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="51.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="51.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" style="15" customWidth="1"/>
-    <col min="2" max="3" width="60.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="51.7109375" style="7"/>
+    <col min="2" max="3" width="60.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="51.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="24" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="24"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="39" t="s">
+      <c r="C3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
+      <c r="B4" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="23"/>
       <c r="E4" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="39" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
+      <c r="B5" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="23"/>
       <c r="E5" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="26"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="25"/>
       <c r="E6" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="32" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="49"/>
+      <c r="B10" s="31" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="55" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="33" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="24" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
       <c r="B15" s="21" t="s">
         <v>62</v>
       </c>
@@ -1766,86 +1750,89 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="21" t="s">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="C16" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
       <c r="B17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="24"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="34" t="s">
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="24"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="34" t="s">
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="24"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54" t="s">
+      <c r="C19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="33" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="24" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="24" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="26"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="24"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="24"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="45"/>
       <c r="B26" s="16" t="s">
         <v>57</v>
@@ -1854,28 +1841,28 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="45"/>
       <c r="B27" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="45"/>
       <c r="B28" s="21" t="s">
         <v>80</v>
       </c>
       <c r="C28" s="20"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="45"/>
       <c r="B29" s="21" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="20"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="45"/>
       <c r="B30" s="18" t="s">
         <v>81</v>
@@ -1884,7 +1871,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="45"/>
       <c r="B31" s="14" t="s">
         <v>82</v>
@@ -1893,141 +1880,133 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="45"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="52" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="45"/>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="46"/>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="38" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="24"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="48"/>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="48"/>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="24"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="48"/>
-      <c r="B39" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="24" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="22"/>
+      <c r="B44" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="22"/>
+      <c r="B45" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="24"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="24"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="24"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B11:B12"/>

</xml_diff>